<commit_message>
Update some mcv info
</commit_message>
<xml_diff>
--- a/GFS_ICBC&SFC.xlsx
+++ b/GFS_ICBC&SFC.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study\Models\dyn_phy_couple_exchange\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE0E944-EF9E-41B7-B163-F138B3217F99}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29640" yWindow="0" windowWidth="25600" windowHeight="19660" tabRatio="500"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Surface" sheetId="1" r:id="rId1"/>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="179">
   <si>
     <t>description</t>
   </si>
@@ -307,246 +313,279 @@
     <t>sfc slope type for lsm ~ slope Dominant category</t>
   </si>
   <si>
+    <t>sea ice thickness</t>
+  </si>
+  <si>
+    <t>canopy water</t>
+  </si>
+  <si>
+    <t>fm parameter from PBL scheme</t>
+  </si>
+  <si>
+    <t>fm at 10m - Ratio of sigma level 1 wind and 10m wind</t>
+  </si>
+  <si>
+    <t>sfc_fld%tprcp - total precipitation</t>
+  </si>
+  <si>
+    <t>sfc_fld%srflag - snow/rain flag for precipitation</t>
+  </si>
+  <si>
+    <t>liquid soil moisture</t>
+  </si>
+  <si>
+    <t>total soil moisture</t>
+  </si>
+  <si>
+    <t>soil temperature (2 layers)</t>
+  </si>
+  <si>
+    <t>water equiv of accumulated snow depth (kg/m**2) over land and sea ice</t>
+  </si>
+  <si>
+    <t>2 meter temperature</t>
+  </si>
+  <si>
+    <t>2 meter humidity</t>
+  </si>
+  <si>
+    <t>global_slmask.t126.grb</t>
+  </si>
+  <si>
+    <t>global_sstclim.2x2.grb</t>
+  </si>
+  <si>
+    <t>global_snoclim.1.875.grb</t>
+  </si>
+  <si>
+    <t>global_zorclim.1x1.grb</t>
+  </si>
+  <si>
+    <t>global_snoalb.1x1.grb</t>
+  </si>
+  <si>
+    <t>global_albedo4.1x1.grb or global_albedo4.1x1.grb</t>
+  </si>
+  <si>
+    <t>global_slope.1x1.grb</t>
+  </si>
+  <si>
+    <t>global_shdmin.0.144x0.144.grb</t>
+  </si>
+  <si>
+    <t>global_shdmax.0.144x0.144.grb</t>
+  </si>
+  <si>
+    <t>global_tg3clim.2.6x1.5.grb</t>
+  </si>
+  <si>
+    <t>global_vegfrac.1x1.grb</t>
+  </si>
+  <si>
+    <t>global_vegtype.1x1.grb</t>
+  </si>
+  <si>
+    <t>global_soiltype.1x1.grb</t>
+  </si>
+  <si>
+    <t>global_soilmcpc.1x1.grb</t>
+  </si>
+  <si>
+    <t>WRF geog files</t>
+  </si>
+  <si>
+    <t>orogwd*</t>
+  </si>
+  <si>
+    <t>maxsnowalb*</t>
+  </si>
+  <si>
+    <t>islope*</t>
+  </si>
+  <si>
+    <t>topo*</t>
+  </si>
+  <si>
+    <t>soiltemp_1deg</t>
+  </si>
+  <si>
+    <t>FNL grib2</t>
+  </si>
+  <si>
+    <t>mcv_input</t>
+  </si>
+  <si>
+    <t>phii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prsi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">phil </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prsl </t>
+  </si>
+  <si>
+    <t>prslk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pgr  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ugrs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">vgrs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">vvl  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tgrs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qgrs </t>
+  </si>
+  <si>
+    <t>interface geopotential height</t>
+  </si>
+  <si>
+    <t>model level pressure in Pa</t>
+  </si>
+  <si>
+    <t>layer geopotential height</t>
+  </si>
+  <si>
+    <t>model layer mean pressure Pa</t>
+  </si>
+  <si>
+    <t>exner function = (p/p0)**rocp</t>
+  </si>
+  <si>
+    <t>surface pressure (Pa) real</t>
+  </si>
+  <si>
+    <t>u component of layer wind</t>
+  </si>
+  <si>
+    <t>v component of layer wind</t>
+  </si>
+  <si>
+    <t>layer mean vertical velocity in pa/sec</t>
+  </si>
+  <si>
+    <t>model layer mean temperature in k</t>
+  </si>
+  <si>
+    <t>layer mean tracer concentration</t>
+  </si>
+  <si>
+    <t>sgh or sgh30</t>
+  </si>
+  <si>
+    <t>see 10-23</t>
+  </si>
+  <si>
+    <t>n x number_of_soil_layers (2)</t>
+  </si>
+  <si>
+    <t>forecast hour parameter from PBL scheme</t>
+  </si>
+  <si>
+    <t>deep soil temperature (at 500cm)</t>
+  </si>
+  <si>
+    <t>TMP_P0_L1_GLL0</t>
+  </si>
+  <si>
+    <t>TSOIL_P0_2L106_GLL0 (4)</t>
+  </si>
+  <si>
+    <t>SOILW_P0_2L106_GLL0 (4)?</t>
+  </si>
+  <si>
+    <t>LANDN_P0_L1_GLL0</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>WEASD_P0_L1_GLL0</t>
+  </si>
+  <si>
+    <t>GFS_FV3</t>
+  </si>
+  <si>
+    <t>fv_land.res</t>
+  </si>
+  <si>
+    <t>landFraction</t>
+  </si>
+  <si>
+    <t>uustar</t>
+  </si>
+  <si>
+    <t>mg_drag.res</t>
+  </si>
+  <si>
+    <t>topoPoint</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>t2m</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>q2m</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>sgh</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>orography (land fraction)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
     <t>unfiltered orography</t>
-  </si>
-  <si>
-    <t>sea ice thickness</t>
-  </si>
-  <si>
-    <t>canopy water</t>
-  </si>
-  <si>
-    <t>fm parameter from PBL scheme</t>
-  </si>
-  <si>
-    <t>fm at 10m - Ratio of sigma level 1 wind and 10m wind</t>
-  </si>
-  <si>
-    <t>sfc_fld%tprcp - total precipitation</t>
-  </si>
-  <si>
-    <t>sfc_fld%srflag - snow/rain flag for precipitation</t>
-  </si>
-  <si>
-    <t>liquid soil moisture</t>
-  </si>
-  <si>
-    <t>total soil moisture</t>
-  </si>
-  <si>
-    <t>soil temperature (2 layers)</t>
-  </si>
-  <si>
-    <t>water equiv of accumulated snow depth (kg/m**2) over land and sea ice</t>
-  </si>
-  <si>
-    <t>2 meter temperature</t>
-  </si>
-  <si>
-    <t>2 meter humidity</t>
-  </si>
-  <si>
-    <t>global_slmask.t126.grb</t>
-  </si>
-  <si>
-    <t>global_sstclim.2x2.grb</t>
-  </si>
-  <si>
-    <t>global_snoclim.1.875.grb</t>
-  </si>
-  <si>
-    <t>global_zorclim.1x1.grb</t>
-  </si>
-  <si>
-    <t>global_snoalb.1x1.grb</t>
-  </si>
-  <si>
-    <t>global_albedo4.1x1.grb or global_albedo4.1x1.grb</t>
-  </si>
-  <si>
-    <t>global_slope.1x1.grb</t>
-  </si>
-  <si>
-    <t>global_shdmin.0.144x0.144.grb</t>
-  </si>
-  <si>
-    <t>global_shdmax.0.144x0.144.grb</t>
-  </si>
-  <si>
-    <t>global_tg3clim.2.6x1.5.grb</t>
-  </si>
-  <si>
-    <t>global_vegfrac.1x1.grb</t>
-  </si>
-  <si>
-    <t>global_vegtype.1x1.grb</t>
-  </si>
-  <si>
-    <t>global_soiltype.1x1.grb</t>
-  </si>
-  <si>
-    <t>global_soilmcpc.1x1.grb</t>
-  </si>
-  <si>
-    <t>WRF geog files</t>
-  </si>
-  <si>
-    <t>orogwd*</t>
-  </si>
-  <si>
-    <t>maxsnowalb*</t>
-  </si>
-  <si>
-    <t>islope*</t>
-  </si>
-  <si>
-    <t>topo*</t>
-  </si>
-  <si>
-    <t>soiltemp_1deg</t>
-  </si>
-  <si>
-    <t>FNL grib2</t>
-  </si>
-  <si>
-    <t>mcv_input</t>
-  </si>
-  <si>
-    <t>phii</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prsi </t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>p</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>exner</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>u_cube</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>v_cube</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exner function at interface</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>prsik</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phil </t>
-  </si>
-  <si>
-    <t xml:space="preserve">prsl </t>
-  </si>
-  <si>
-    <t>prslk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pgr  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ugrs </t>
-  </si>
-  <si>
-    <t xml:space="preserve">vgrs </t>
-  </si>
-  <si>
-    <t xml:space="preserve">vvl  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tgrs </t>
-  </si>
-  <si>
-    <t xml:space="preserve">qgrs </t>
-  </si>
-  <si>
-    <t>interface geopotential height</t>
-  </si>
-  <si>
-    <t>model level pressure in Pa</t>
-  </si>
-  <si>
-    <t>Exner function at interface</t>
-  </si>
-  <si>
-    <t>layer geopotential height</t>
-  </si>
-  <si>
-    <t>model layer mean pressure Pa</t>
-  </si>
-  <si>
-    <t>exner function = (p/p0)**rocp</t>
-  </si>
-  <si>
-    <t>surface pressure (Pa) real</t>
-  </si>
-  <si>
-    <t>u component of layer wind</t>
-  </si>
-  <si>
-    <t>v component of layer wind</t>
-  </si>
-  <si>
-    <t>layer mean vertical velocity in pa/sec</t>
-  </si>
-  <si>
-    <t>model layer mean temperature in k</t>
-  </si>
-  <si>
-    <t>layer mean tracer concentration</t>
-  </si>
-  <si>
-    <t>sgh or sgh30</t>
-  </si>
-  <si>
-    <t>see 10-23</t>
-  </si>
-  <si>
-    <t>topoCell or topoPoint</t>
-  </si>
-  <si>
-    <t>n x number_of_soil_layers (2)</t>
-  </si>
-  <si>
-    <t>forecast hour parameter from PBL scheme</t>
-  </si>
-  <si>
-    <t>deep soil temperature (at 500cm)</t>
-  </si>
-  <si>
-    <t>TMP_P0_L1_GLL0</t>
-  </si>
-  <si>
-    <t>TSOIL_P0_2L106_GLL0 (4)</t>
-  </si>
-  <si>
-    <t>SOILW_P0_2L106_GLL0 (4)?</t>
-  </si>
-  <si>
-    <t>LANDN_P0_L1_GLL0</t>
-  </si>
-  <si>
-    <t>v</t>
-  </si>
-  <si>
-    <t>WEASD_P0_L1_GLL0</t>
-  </si>
-  <si>
-    <t>GFS_FV3</t>
-  </si>
-  <si>
-    <t>fv_land.res</t>
-  </si>
-  <si>
-    <t>orography (land fraction)</t>
-  </si>
-  <si>
-    <t>landFraction</t>
-  </si>
-  <si>
-    <t>uustar</t>
-  </si>
-  <si>
-    <t>mg_drag.res</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -554,7 +593,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -562,14 +601,14 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -577,8 +616,15 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -650,52 +696,60 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="42" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1020,25 +1074,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.3" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.84765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.34765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.1484375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1484375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.1484375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.84765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1055,16 +1110,16 @@
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -1075,13 +1130,13 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -1092,13 +1147,13 @@
         <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -1109,7 +1164,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -1120,10 +1175,10 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -1134,10 +1189,10 @@
         <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -1148,7 +1203,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -1159,13 +1214,13 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="H8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>13</v>
       </c>
@@ -1173,10 +1228,10 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>20</v>
       </c>
@@ -1187,10 +1242,10 @@
         <v>33</v>
       </c>
       <c r="H10" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>23</v>
       </c>
@@ -1201,7 +1256,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>24</v>
       </c>
@@ -1212,10 +1267,10 @@
         <v>32</v>
       </c>
       <c r="F12" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>25</v>
       </c>
@@ -1226,10 +1281,10 @@
         <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>26</v>
       </c>
@@ -1240,10 +1295,10 @@
         <v>37</v>
       </c>
       <c r="F14" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>27</v>
       </c>
@@ -1254,10 +1309,10 @@
         <v>38</v>
       </c>
       <c r="F15" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
         <v>28</v>
       </c>
@@ -1268,10 +1323,10 @@
         <v>35</v>
       </c>
       <c r="F16" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
         <v>29</v>
       </c>
@@ -1282,10 +1337,10 @@
         <v>39</v>
       </c>
       <c r="F17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>30</v>
       </c>
@@ -1296,10 +1351,10 @@
         <v>40</v>
       </c>
       <c r="F18" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>31</v>
       </c>
@@ -1310,10 +1365,10 @@
         <v>41</v>
       </c>
       <c r="F19" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>43</v>
       </c>
@@ -1324,7 +1379,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>44</v>
       </c>
@@ -1335,7 +1390,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
         <v>45</v>
       </c>
@@ -1346,7 +1401,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
         <v>46</v>
       </c>
@@ -1357,7 +1412,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
         <v>50</v>
       </c>
@@ -1368,7 +1423,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
         <v>52</v>
       </c>
@@ -1379,13 +1434,13 @@
         <v>53</v>
       </c>
       <c r="E25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F25" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
         <v>54</v>
       </c>
@@ -1396,10 +1451,10 @@
         <v>82</v>
       </c>
       <c r="E26" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
         <v>55</v>
       </c>
@@ -1410,10 +1465,10 @@
         <v>83</v>
       </c>
       <c r="E27" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>56</v>
       </c>
@@ -1424,10 +1479,10 @@
         <v>84</v>
       </c>
       <c r="E28" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
         <v>57</v>
       </c>
@@ -1438,10 +1493,10 @@
         <v>85</v>
       </c>
       <c r="E29" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
         <v>58</v>
       </c>
@@ -1452,10 +1507,10 @@
         <v>86</v>
       </c>
       <c r="E30" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
         <v>59</v>
       </c>
@@ -1466,10 +1521,10 @@
         <v>87</v>
       </c>
       <c r="E31" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B32" t="s">
         <v>60</v>
       </c>
@@ -1480,13 +1535,13 @@
         <v>94</v>
       </c>
       <c r="E32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F32" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B33" t="s">
         <v>61</v>
       </c>
@@ -1497,10 +1552,10 @@
         <v>88</v>
       </c>
       <c r="E33" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B34" t="s">
         <v>62</v>
       </c>
@@ -1511,10 +1566,10 @@
         <v>89</v>
       </c>
       <c r="E34" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B35" t="s">
         <v>63</v>
       </c>
@@ -1522,13 +1577,13 @@
         <v>21</v>
       </c>
       <c r="D35" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E35" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B36" t="s">
         <v>64</v>
       </c>
@@ -1539,10 +1594,10 @@
         <v>90</v>
       </c>
       <c r="E36" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B37" t="s">
         <v>65</v>
       </c>
@@ -1553,10 +1608,10 @@
         <v>91</v>
       </c>
       <c r="E37" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B38" t="s">
         <v>66</v>
       </c>
@@ -1567,12 +1622,12 @@
         <v>92</v>
       </c>
       <c r="E38" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B39" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C39" t="s">
         <v>21</v>
@@ -1581,7 +1636,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="2:8">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B40" t="s">
         <v>67</v>
       </c>
@@ -1589,16 +1644,16 @@
         <v>21</v>
       </c>
       <c r="D40" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E40" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B41" t="s">
         <v>68</v>
       </c>
@@ -1606,16 +1661,16 @@
         <v>21</v>
       </c>
       <c r="D41" t="s">
-        <v>95</v>
+        <v>172</v>
       </c>
       <c r="F41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H41" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B42" t="s">
         <v>69</v>
       </c>
@@ -1623,10 +1678,10 @@
         <v>21</v>
       </c>
       <c r="D42" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B43" t="s">
         <v>70</v>
       </c>
@@ -1634,13 +1689,13 @@
         <v>21</v>
       </c>
       <c r="D43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G43" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B44" t="s">
         <v>71</v>
       </c>
@@ -1648,10 +1703,10 @@
         <v>21</v>
       </c>
       <c r="D44" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B45" t="s">
         <v>72</v>
       </c>
@@ -1659,10 +1714,10 @@
         <v>21</v>
       </c>
       <c r="D45" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B46" t="s">
         <v>73</v>
       </c>
@@ -1670,10 +1725,10 @@
         <v>21</v>
       </c>
       <c r="D46" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B47" t="s">
         <v>75</v>
       </c>
@@ -1681,10 +1736,10 @@
         <v>21</v>
       </c>
       <c r="D47" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B48" t="s">
         <v>74</v>
       </c>
@@ -1692,10 +1747,10 @@
         <v>21</v>
       </c>
       <c r="D48" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B49" t="s">
         <v>76</v>
       </c>
@@ -1703,58 +1758,58 @@
         <v>21</v>
       </c>
       <c r="D49" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B50" t="s">
         <v>77</v>
       </c>
       <c r="C50" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G50" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="51" spans="2:7">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B51" t="s">
         <v>78</v>
       </c>
       <c r="C51" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E51" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G51" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="52" spans="2:7">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B52" t="s">
         <v>79</v>
       </c>
       <c r="C52" t="s">
+        <v>153</v>
+      </c>
+      <c r="D52" t="s">
+        <v>103</v>
+      </c>
+      <c r="F52" t="s">
+        <v>126</v>
+      </c>
+      <c r="G52" t="s">
         <v>157</v>
       </c>
-      <c r="D52" t="s">
-        <v>104</v>
-      </c>
-      <c r="F52" t="s">
-        <v>127</v>
-      </c>
-      <c r="G52" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="53" spans="2:7">
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B53" t="s">
         <v>80</v>
       </c>
@@ -1762,10 +1817,13 @@
         <v>21</v>
       </c>
       <c r="D53" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="54" spans="2:7">
+        <v>105</v>
+      </c>
+      <c r="H53" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B54" t="s">
         <v>81</v>
       </c>
@@ -1773,10 +1831,14 @@
         <v>21</v>
       </c>
       <c r="D54" t="s">
-        <v>107</v>
+        <v>106</v>
+      </c>
+      <c r="H54" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -1788,21 +1850,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.3" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.84765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.34765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1816,149 +1879,163 @@
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
         <v>130</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" t="s">
+        <v>160</v>
+      </c>
+      <c r="G3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4" t="s">
+        <v>177</v>
+      </c>
+      <c r="F4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" t="s">
         <v>142</v>
       </c>
-      <c r="F2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="B3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" t="s">
         <v>143</v>
       </c>
-      <c r="F3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="B4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="F6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" t="s">
         <v>144</v>
       </c>
-      <c r="F4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="B5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="F7" t="s">
+        <v>160</v>
+      </c>
+      <c r="G7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" t="s">
         <v>145</v>
       </c>
-      <c r="F5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="B6" t="s">
-        <v>134</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="F8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" t="s">
         <v>146</v>
       </c>
-      <c r="F6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="B7" t="s">
-        <v>135</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="F9" t="s">
+        <v>160</v>
+      </c>
+      <c r="G9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" t="s">
         <v>147</v>
       </c>
-      <c r="F7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="B8" t="s">
-        <v>136</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="F10" t="s">
+        <v>160</v>
+      </c>
+      <c r="G10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11" t="s">
         <v>148</v>
       </c>
-      <c r="F8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="B9" t="s">
-        <v>137</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="F11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" t="s">
         <v>149</v>
       </c>
-      <c r="F9" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="B10" t="s">
-        <v>138</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="F12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>139</v>
+      </c>
+      <c r="D13" t="s">
         <v>150</v>
       </c>
-      <c r="F10" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="B11" t="s">
-        <v>139</v>
-      </c>
-      <c r="D11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F11" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="B12" t="s">
-        <v>140</v>
-      </c>
-      <c r="D12" t="s">
-        <v>152</v>
-      </c>
-      <c r="F12" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="B13" t="s">
-        <v>141</v>
-      </c>
-      <c r="D13" t="s">
-        <v>153</v>
-      </c>
       <c r="F13" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>